<commit_message>
Uploaded on 13-06-16 at 8.40pm
</commit_message>
<xml_diff>
--- a/assets/excel/Phone.xlsx
+++ b/assets/excel/Phone.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="14295" windowHeight="4620"/>
+    <workbookView xWindow="480" yWindow="360" windowWidth="19815" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,63 +16,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="4">
   <si>
-    <t>(123) 456 7899</t>
+    <t>Phone Number</t>
   </si>
   <si>
-    <t>(123)-456-7899</t>
-  </si>
-  <si>
-    <t>(123).456.789</t>
-  </si>
-  <si>
-    <t>(123)-456 7899</t>
-  </si>
-  <si>
-    <t>(123)-456.7899</t>
-  </si>
-  <si>
-    <t>(123).456-7899</t>
-  </si>
-  <si>
-    <t>(123).</t>
-  </si>
-  <si>
-    <t>(123).456</t>
-  </si>
-  <si>
-    <t>(123).456.78</t>
-  </si>
-  <si>
-    <t>(123).4567899</t>
-  </si>
-  <si>
-    <t>(123)-</t>
-  </si>
-  <si>
-    <t>(123)-456</t>
-  </si>
-  <si>
-    <t>(123)-456.</t>
-  </si>
-  <si>
-    <t>123-456-7899</t>
-  </si>
-  <si>
-    <t>123.456.7899</t>
-  </si>
-  <si>
-    <t>123-456.7899</t>
-  </si>
-  <si>
-    <t>123.456-7899</t>
-  </si>
-  <si>
-    <t>123-456</t>
-  </si>
-  <si>
-    <t>Phone Numbers</t>
+    <t>Result</t>
   </si>
   <si>
     <t>Valid</t>
@@ -80,18 +29,12 @@
   <si>
     <t>Invalid</t>
   </si>
-  <si>
-    <t>Verified</t>
-  </si>
-  <si>
-    <t>(144) 452 2563</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -100,39 +43,20 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF00B050"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="9" tint="-0.249977111117893"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.499984740745262"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -147,11 +71,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,193 +377,852 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B110"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75">
-      <c r="A1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>21</v>
+    <row r="1" spans="1:2" s="4" customFormat="1">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>19</v>
+      <c r="A2" s="2">
+        <v>9737614994</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>19</v>
+      <c r="A3" s="2">
+        <v>9737614994</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4">
-        <v>1234567899</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>20</v>
+      <c r="A4" s="2">
+        <v>9737633478</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>20</v>
+      <c r="A5" s="2">
+        <v>9737633478</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>20</v>
+      <c r="A6" s="2">
+        <v>9737633775</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>20</v>
+      <c r="A7" s="2">
+        <v>9179020676</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>20</v>
+      <c r="A8" s="2">
+        <v>9179020676</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>20</v>
+      <c r="A9" s="2">
+        <v>9082323756</v>
+      </c>
+      <c r="B9" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>20</v>
+      <c r="A10" s="2">
+        <v>9086543191</v>
+      </c>
+      <c r="B10" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>20</v>
+      <c r="A11" s="2">
+        <v>9086543191</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>20</v>
+      <c r="A12" s="2">
+        <v>6318219408</v>
+      </c>
+      <c r="B12" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>19</v>
+      <c r="A13" s="2">
+        <v>9737615768</v>
+      </c>
+      <c r="B13" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>20</v>
+      <c r="A14" s="2">
+        <v>9737615768</v>
+      </c>
+      <c r="B14" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>20</v>
+      <c r="A15" s="2">
+        <v>9737615768</v>
+      </c>
+      <c r="B15" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>20</v>
+      <c r="A16" s="2">
+        <v>9082321379</v>
+      </c>
+      <c r="B16" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>20</v>
+      <c r="A17" s="2">
+        <v>9082322783</v>
+      </c>
+      <c r="B17" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>20</v>
+      <c r="A18" s="2">
+        <v>9735098549</v>
+      </c>
+      <c r="B18" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>20</v>
+      <c r="A19" s="2">
+        <v>9738783542</v>
+      </c>
+      <c r="B19" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" t="s">
-        <v>16</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>20</v>
+      <c r="A20" s="2">
+        <v>9738783542</v>
+      </c>
+      <c r="B20" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21">
-        <v>123.456</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>20</v>
+      <c r="A21" s="2">
+        <v>9082331297</v>
+      </c>
+      <c r="B21" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" t="s">
-        <v>17</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>20</v>
-      </c>
+      <c r="A22" s="2">
+        <v>9083175629</v>
+      </c>
+      <c r="B22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="2">
+        <v>9087890436</v>
+      </c>
+      <c r="B23" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="2">
+        <v>9082321225</v>
+      </c>
+      <c r="B24" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="2">
+        <v>9082321225</v>
+      </c>
+      <c r="B25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="2">
+        <v>9089175637</v>
+      </c>
+      <c r="B26" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="2">
+        <v>9089175637</v>
+      </c>
+      <c r="B27" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="2">
+        <v>9737314358</v>
+      </c>
+      <c r="B28" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="2">
+        <v>9082332516</v>
+      </c>
+      <c r="B29" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="2">
+        <v>9736998661</v>
+      </c>
+      <c r="B30" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="2">
+        <v>9737315041</v>
+      </c>
+      <c r="B31" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="2">
+        <v>9737315041</v>
+      </c>
+      <c r="B32" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="2">
+        <v>9086048617</v>
+      </c>
+      <c r="B33" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="2">
+        <v>9086478580</v>
+      </c>
+      <c r="B34" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="2">
+        <v>9086478580</v>
+      </c>
+      <c r="B35" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="2">
+        <v>9086478580</v>
+      </c>
+      <c r="B36" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="2">
+        <v>9082334021</v>
+      </c>
+      <c r="B37" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="2">
+        <v>7323883631</v>
+      </c>
+      <c r="B38" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="2">
+        <v>7323883631</v>
+      </c>
+      <c r="B39" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="2">
+        <v>9087553142</v>
+      </c>
+      <c r="B40" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="2">
+        <v>9087698415</v>
+      </c>
+      <c r="B41" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="2">
+        <v>9082227416</v>
+      </c>
+      <c r="B42" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="2">
+        <v>9082227416</v>
+      </c>
+      <c r="B43" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="2">
+        <v>9082331429</v>
+      </c>
+      <c r="B44" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="2">
+        <v>9087552104</v>
+      </c>
+      <c r="B45" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" s="2">
+        <v>9087552104</v>
+      </c>
+      <c r="B46" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="2">
+        <v>9083550196</v>
+      </c>
+      <c r="B47" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="2">
+        <v>9083550196</v>
+      </c>
+      <c r="B48" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="2">
+        <v>9082334616</v>
+      </c>
+      <c r="B49" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" s="2">
+        <v>9082648408</v>
+      </c>
+      <c r="B50" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" s="2">
+        <v>9087551982</v>
+      </c>
+      <c r="B51" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="2">
+        <v>9087551982</v>
+      </c>
+      <c r="B52" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="2">
+        <v>9087898356</v>
+      </c>
+      <c r="B53" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" s="2">
+        <v>9087898356</v>
+      </c>
+      <c r="B54" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" s="2">
+        <v>9082334411</v>
+      </c>
+      <c r="B55" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="2">
+        <v>9089304598</v>
+      </c>
+      <c r="B56" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="2">
+        <v>7322597422</v>
+      </c>
+      <c r="B57" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="2">
+        <v>7322597422</v>
+      </c>
+      <c r="B58" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="2">
+        <v>7322595485</v>
+      </c>
+      <c r="B59" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="2">
+        <v>9734837901</v>
+      </c>
+      <c r="B60" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" s="2">
+        <v>7323828654</v>
+      </c>
+      <c r="B61" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" s="2">
+        <v>7323829740</v>
+      </c>
+      <c r="B62" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" s="2">
+        <v>9082330893</v>
+      </c>
+      <c r="B63" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" s="2">
+        <v>9082333786</v>
+      </c>
+      <c r="B64" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" s="2">
+        <v>9082940986</v>
+      </c>
+      <c r="B65" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" s="2">
+        <v>9082332174</v>
+      </c>
+      <c r="B66" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" s="2">
+        <v>9082330516</v>
+      </c>
+      <c r="B67" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" s="2">
+        <v>9087557779</v>
+      </c>
+      <c r="B68" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" s="2">
+        <v>9087557779</v>
+      </c>
+      <c r="B69" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" s="2">
+        <v>9087892599</v>
+      </c>
+      <c r="B70" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" s="2">
+        <v>9082797094</v>
+      </c>
+      <c r="B71" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" s="2">
+        <v>9085615914</v>
+      </c>
+      <c r="B72" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" s="2">
+        <v>9082323612</v>
+      </c>
+      <c r="B73" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" s="2">
+        <v>6464183508</v>
+      </c>
+      <c r="B74" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" s="2">
+        <v>9086543761</v>
+      </c>
+      <c r="B75" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" s="2">
+        <v>9086541387</v>
+      </c>
+      <c r="B76" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" s="2">
+        <v>9086541387</v>
+      </c>
+      <c r="B77" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" s="2">
+        <v>9087975140</v>
+      </c>
+      <c r="B78" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" s="2">
+        <v>7323887932</v>
+      </c>
+      <c r="B79" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" s="2">
+        <v>9083805381</v>
+      </c>
+      <c r="B80" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" s="2">
+        <v>7323881594</v>
+      </c>
+      <c r="B81" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" s="2">
+        <v>7323881594</v>
+      </c>
+      <c r="B82" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" s="2">
+        <v>7323881594</v>
+      </c>
+      <c r="B83" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" s="2">
+        <v>9083172811</v>
+      </c>
+      <c r="B84" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" s="2">
+        <v>9083172811</v>
+      </c>
+      <c r="B85" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" s="2">
+        <v>9082328141</v>
+      </c>
+      <c r="B86" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" s="2">
+        <v>9086546274</v>
+      </c>
+      <c r="B87" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" s="2">
+        <v>9083890399</v>
+      </c>
+      <c r="B88" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" s="2">
+        <v>9083890399</v>
+      </c>
+      <c r="B89" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" s="2">
+        <v>9082321963</v>
+      </c>
+      <c r="B90" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" s="2">
+        <v>9083105863</v>
+      </c>
+      <c r="B91" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" s="2">
+        <v>9087564654</v>
+      </c>
+      <c r="B92" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" s="2">
+        <v>9087564654</v>
+      </c>
+      <c r="B93" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" s="2">
+        <v>9087564654</v>
+      </c>
+      <c r="B94" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" s="2">
+        <v>9082321275</v>
+      </c>
+      <c r="B95" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" s="2">
+        <v>9082321275</v>
+      </c>
+      <c r="B96" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" s="2">
+        <v>9088890762</v>
+      </c>
+      <c r="B97" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" s="2">
+        <v>9088890762</v>
+      </c>
+      <c r="B98" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99" s="2">
+        <v>9088890762</v>
+      </c>
+      <c r="B99" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100" s="2">
+        <v>9087895953</v>
+      </c>
+      <c r="B100" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" s="2">
+        <v>9088894117</v>
+      </c>
+      <c r="B101" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102" s="2"/>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" s="2"/>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" s="2"/>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105" s="2"/>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106" s="2"/>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107" s="2"/>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108" s="2"/>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="A109" s="2"/>
+    </row>
+    <row r="110" spans="1:2">
+      <c r="A110" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>